<commit_message>
q learning finally fonctional with every environments, wouhou
</commit_message>
<xml_diff>
--- a/environments/results.xlsx
+++ b/environments/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,41 @@
           <t>Environnement</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Stat - alpha</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Stat - epsilon</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Stat - episodes</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Hyper - alpha</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Hyper - epsilon</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Hyper - episodes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-15 04:23:30</t>
+          <t>2025-06-15 19:08:20</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -466,11 +496,17 @@
           <t>{'win': 1, 'loss': 0, 'draw': 1}</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-06-15 04:23:43</t>
+          <t>2025-06-15 19:08:24</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -480,14 +516,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'win': 2, 'loss': 1, 'draw': 1}</t>
-        </is>
-      </c>
+          <t>{'win': 2, 'loss': 0, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-06-15 04:23:47</t>
+          <t>2025-06-15 19:08:27</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -497,14 +539,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'win': 4, 'loss': 1, 'draw': 1}</t>
-        </is>
-      </c>
+          <t>{'win': 2, 'loss': 0, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-06-15 04:23:50</t>
+          <t>2025-06-15 19:57:47</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -514,14 +562,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'win': 4, 'loss': 1, 'draw': 3}</t>
-        </is>
+          <t>{'win': 2, 'loss': 0, 'draw': 0}</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-06-15 04:23:52</t>
+          <t>2025-06-15 19:57:54</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -531,14 +597,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'win': 5, 'loss': 1, 'draw': 4}</t>
-        </is>
+          <t>{'win': 2, 'loss': 0, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-06-15 04:23:54</t>
+          <t>2025-06-15 19:57:59</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -548,14 +632,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'win': 6, 'loss': 2, 'draw': 4}</t>
-        </is>
+          <t>{'win': 2, 'loss': 0, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-06-15 04:26:54</t>
+          <t>2025-06-15 19:58:03</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -565,25 +667,26 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'win': 0, 'loss': 1, 'draw': 1}</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2025-06-15 04:26:58</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Q Learning</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{'win': 0, 'loss': 2, 'draw': 2}</t>
-        </is>
+          <t>{'win': 3, 'loss': 0, 'draw': 5}</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
q-learning fonctional with each environnment
</commit_message>
<xml_diff>
--- a/environments/results.xlsx
+++ b/environments/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,6 +689,121 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:52:57</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Q Learning</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:53:04</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Q Learning</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 1, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:53:07</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Q Learning</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 2, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:53:10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Q Learning</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 2, 'draw': 3}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-06-25 17:53:44</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Joueur Humain</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
q learning policy and value iteration fonctional in each environments
</commit_message>
<xml_diff>
--- a/environments/results.xlsx
+++ b/environments/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -804,6 +804,282 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:34:11</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Policy Iteration</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 1, 'draw': 0}</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:34:20</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Policy Iteration</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 2, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:34:22</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Policy Iteration</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 2, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:35:09</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Policy Iteration</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 0, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:35:13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Policy Iteration</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 3}</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:35:17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Policy Iteration</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 5}</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:47:15</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Value Iteration</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:47:20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Value Iteration</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 2, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:47:23</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Value Iteration</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 2, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:47:28</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Value Iteration</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 2, 'draw': 3}</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:47:31</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Value Iteration</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'win': 4, 'loss': 2, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-06-25 19:48:24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Joueur Humain</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 1, 'draw': 0}</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
policy value iteration dyna q dynaq+ sarsa expected sarsa qlearning first visite MC fonctional in each environment but dyna q dyna q+ sarsa expected sarsa et first visite mc thes agents directs towards -1 in line world and yet I dont know why
</commit_message>
<xml_diff>
--- a/environments/results.xlsx
+++ b/environments/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,26 @@
           <t>Hyper - episodes</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Stat - planning_steps</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Stat - kappa</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Hyper - planning_steps</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Hyper - kappa</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -502,6 +522,10 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -525,6 +549,10 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -548,6 +576,10 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -583,6 +615,10 @@
       <c r="I5" t="n">
         <v>1000</v>
       </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -618,6 +654,10 @@
       <c r="I6" t="n">
         <v>1000</v>
       </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -653,6 +693,10 @@
       <c r="I7" t="n">
         <v>1000</v>
       </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -688,6 +732,10 @@
       <c r="I8" t="n">
         <v>1000</v>
       </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -711,6 +759,10 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -734,6 +786,10 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -757,6 +813,10 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -780,6 +840,10 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -803,6 +867,10 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -826,6 +894,10 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -849,6 +921,10 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -872,6 +948,10 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -895,6 +975,10 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -918,6 +1002,10 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -941,6 +1029,10 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -964,6 +1056,10 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -987,6 +1083,10 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1010,6 +1110,10 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1033,6 +1137,10 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1056,6 +1164,10 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1079,6 +1191,1159 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:57:15</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 0, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:57:19</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 3}</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:57:23</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 1, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:57:26</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 2, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:57:28</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 2, 'draw': 5}</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:59:47</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:59:51</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 3}</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:59:53</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 5}</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:59:55</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 1, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-06-26 01:59:56</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Dyna Q</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 2, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:12:22</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="n">
+        <v>10</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L36" t="n">
+        <v>10</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:12:29</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 1, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="n">
+        <v>10</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L37" t="n">
+        <v>10</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:12:35</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 2, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="n">
+        <v>10</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L38" t="n">
+        <v>10</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:12:39</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 3, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="n">
+        <v>10</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L39" t="n">
+        <v>10</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:12:42</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 3, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="n">
+        <v>10</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L40" t="n">
+        <v>10</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:12:53</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>{'win': 4, 'loss': 4, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="n">
+        <v>10</v>
+      </c>
+      <c r="K41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L41" t="n">
+        <v>10</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:13:48</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Dyna Q+</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:14:07</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Joueur Humain</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 1, 'draw': 0}</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:30</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:36</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 2, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:39</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 3, 'draw': 3}</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:43</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 3, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:45</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 4, 'draw': 5}</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F48" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:46</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 4, 'draw': 7}</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:29:49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Sarsa</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 4, 'draw': 8}</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:11</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 1, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I51" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:19</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 2, 'draw': 2}</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:24</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 2, 'draw': 4}</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:29</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>{'win': 0, 'loss': 2, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:34</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 2, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:38</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'win': 2, 'loss': 4, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:41</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 5, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:43</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>{'win': 3, 'loss': 7, 'draw': 6}</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:55:44</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>First Visit MC</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'win': 4, 'loss': 7, 'draw': 7}</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-06-26 02:56:02</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Joueur Humain</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'win': 1, 'loss': 0, 'draw': 1}</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>